<commit_message>
Data Driven functionality added
</commit_message>
<xml_diff>
--- a/BlogUITests/DataDrivenTests/UserData.xlsx
+++ b/BlogUITests/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
   <si>
     <t>Key</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>rosen</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>CreateNewPost</t>
+  </si>
+  <si>
+    <t>DeletePost</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,6 +671,57 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>123</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>123</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>123</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -671,8 +731,11 @@
     <hyperlink ref="B8" r:id="rId5"/>
     <hyperlink ref="B9" r:id="rId6"/>
     <hyperlink ref="B10" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B13" r:id="rId9"/>
+    <hyperlink ref="B14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Data Driven functionality added"
This reverts commit feeaae5e279a3c0cecf0952fb492b821e60ed714.
</commit_message>
<xml_diff>
--- a/BlogUITests/DataDrivenTests/UserData.xlsx
+++ b/BlogUITests/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Key</t>
   </si>
@@ -74,15 +74,6 @@
   </si>
   <si>
     <t>rosen</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>CreateNewPost</t>
-  </si>
-  <si>
-    <t>DeletePost</t>
   </si>
 </sst>
 </file>
@@ -469,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,57 +662,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1">
-        <v>123</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1">
-        <v>123</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1">
-        <v>123</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -731,11 +671,8 @@
     <hyperlink ref="B8" r:id="rId5"/>
     <hyperlink ref="B9" r:id="rId6"/>
     <hyperlink ref="B10" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New path in accessData class
</commit_message>
<xml_diff>
--- a/BlogUITests/DataDrivenTests/UserData.xlsx
+++ b/BlogUITests/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Key</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>rosen</t>
+  </si>
+  <si>
+    <t>TryToLoggingIn</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E11" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,6 +665,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>123</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -671,8 +691,9 @@
     <hyperlink ref="B8" r:id="rId5"/>
     <hyperlink ref="B9" r:id="rId6"/>
     <hyperlink ref="B10" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Login with Invalid Username Test
</commit_message>
<xml_diff>
--- a/BlogUITests/DataDrivenTests/UserData.xlsx
+++ b/BlogUITests/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>Key</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>TryToLoggingIn</t>
+  </si>
+  <si>
+    <t>sgdfhh</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,12 +617,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -689,11 +692,10 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B9" r:id="rId6"/>
-    <hyperlink ref="B10" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Login With Invalid Username 2
</commit_message>
<xml_diff>
--- a/BlogUITests/DataDrivenTests/UserData.xlsx
+++ b/BlogUITests/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Key</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>TryToLoggingIn</t>
+  </si>
+  <si>
+    <t>kjdfb</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,13 +625,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
-        <v>12345</v>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
@@ -689,7 +695,7 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId6" display="abv@abv.bg"/>
     <hyperlink ref="B10" r:id="rId7"/>
     <hyperlink ref="B12" r:id="rId8"/>
   </hyperlinks>

</xml_diff>